<commit_message>
Added some npm packages
</commit_message>
<xml_diff>
--- a/Players.xlsx
+++ b/Players.xlsx
@@ -3,19 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6CC2133-3AE3-4DFD-B14D-BA82EECE574D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDB2139-1D21-468A-8BA7-17F6E561B2A9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lakers" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Heat" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="asdad" localSheetId="0">Lakers!$N$1:$S$21</definedName>
-    <definedName name="asdad" localSheetId="1">Sheet1!$A$1:$G$22</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,20 +25,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{73198A13-84C5-41DB-845C-C8B1F959F488}" name="asdad" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\Users\TinTin\Desktop\asdad.txt" tab="0" comma="1">
-      <textFields count="7">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="2" xr16:uid="{6ADF788C-C527-4EB5-9C77-A83D33A4C8CE}" name="asdad1" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="1" xr16:uid="{6ADF788C-C527-4EB5-9C77-A83D33A4C8CE}" name="asdad1" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\TinTin\Desktop\asdad.txt" tab="0" comma="1">
       <textFields count="7">
         <textField/>
@@ -56,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="44">
   <si>
     <t>Kentavious Caldwell-Pope</t>
   </si>
@@ -155,81 +141,6 @@
   </si>
   <si>
     <t>6'7</t>
-  </si>
-  <si>
-    <t>FG%</t>
-  </si>
-  <si>
-    <t>FT%</t>
-  </si>
-  <si>
-    <t>TRB</t>
-  </si>
-  <si>
-    <t>AST</t>
-  </si>
-  <si>
-    <t>PTS/G</t>
-  </si>
-  <si>
-    <t>LeBron James\jamesle01</t>
-  </si>
-  <si>
-    <t>Anthony Davis\davisan02</t>
-  </si>
-  <si>
-    <t>Kentavious Caldwell-Pope\caldwke01</t>
-  </si>
-  <si>
-    <t>Kyle Kuzma\kuzmaky01</t>
-  </si>
-  <si>
-    <t>Danny Green\greenda02</t>
-  </si>
-  <si>
-    <t>Avery Bradley\bradlav01</t>
-  </si>
-  <si>
-    <t>Dion Waiters\waitedi01</t>
-  </si>
-  <si>
-    <t>Rajon Rondo\rondora01</t>
-  </si>
-  <si>
-    <t>Dwight Howard\howardw01</t>
-  </si>
-  <si>
-    <t>Alex Caruso\carusal01</t>
-  </si>
-  <si>
-    <t>JaVale McGee\mcgeeja01</t>
-  </si>
-  <si>
-    <t>Markieff Morris\morrima02</t>
-  </si>
-  <si>
-    <t>Talen Horton-Tucker\hortota01</t>
-  </si>
-  <si>
-    <t>J.R. Smith\smithjr01</t>
-  </si>
-  <si>
-    <t>Quinn Cook\cookqu01</t>
-  </si>
-  <si>
-    <t>Troy Daniels\danietr01</t>
-  </si>
-  <si>
-    <t>Devontae Cacok\cacokde01</t>
-  </si>
-  <si>
-    <t>Jared Dudley\dudleja01</t>
-  </si>
-  <si>
-    <t>Kostas Antetokounmpo\antetko01</t>
-  </si>
-  <si>
-    <t>Zach Norvell\norveza01</t>
   </si>
   <si>
     <t>personalfouls</t>
@@ -325,11 +236,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="asdad" connectionId="2" xr16:uid="{2F210347-C746-4B9C-8938-614F4991F7C4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="asdad" connectionId="1" xr16:uid="{BC64F41B-608F-4C8E-AD93-9E15536958EE}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="asdad" connectionId="1" xr16:uid="{2F210347-C746-4B9C-8938-614F4991F7C4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -595,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,7 +516,7 @@
     <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="6" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="4.28515625" bestFit="1" customWidth="1"/>
@@ -617,40 +524,40 @@
     <col min="19" max="19" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -682,8 +589,20 @@
         <v>1.9</v>
       </c>
       <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <f>ROUNDUP(H2,0)*10</f>
+        <v>30</v>
+      </c>
+      <c r="M2">
+        <f>ROUNDUP(I2,0)*10</f>
+        <v>20</v>
+      </c>
+      <c r="N2">
+        <f>ROUNDUP(J2,0)*10</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -715,8 +634,20 @@
         <v>3.2</v>
       </c>
       <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <f t="shared" ref="L3:L20" si="0">ROUNDUP(H3,0)*10</f>
+        <v>80</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M20" si="1">ROUNDUP(I3,0)*10</f>
+        <v>10</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N20" si="2">ROUNDUP(J3,0)*10</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -745,11 +676,23 @@
         <v>1.3</v>
       </c>
       <c r="J4">
-        <v>2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -778,11 +721,23 @@
         <v>0.5</v>
       </c>
       <c r="J5">
-        <v>2.2999999999999998</v>
+        <v>1.8</v>
       </c>
       <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -811,11 +766,23 @@
         <v>10.199999999999999</v>
       </c>
       <c r="J6">
-        <v>1.8</v>
+        <v>1.5</v>
       </c>
       <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -844,11 +811,23 @@
         <v>1.9</v>
       </c>
       <c r="J7">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -877,11 +856,23 @@
         <v>3.2</v>
       </c>
       <c r="J8">
-        <v>2.5</v>
+        <v>2.1</v>
       </c>
       <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -910,11 +901,23 @@
         <v>1.3</v>
       </c>
       <c r="J9">
-        <v>2.1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -943,11 +946,23 @@
         <v>1.3</v>
       </c>
       <c r="J10">
-        <v>2.2000000000000002</v>
+        <v>1.2</v>
       </c>
       <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -976,11 +991,23 @@
         <v>5</v>
       </c>
       <c r="J11">
-        <v>1.2</v>
+        <v>0.9</v>
       </c>
       <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
@@ -1009,11 +1036,23 @@
         <v>0.6</v>
       </c>
       <c r="J12">
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
       <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -1042,11 +1081,23 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="J13">
-        <v>0.6</v>
+        <v>2.1</v>
       </c>
       <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
@@ -1075,11 +1126,23 @@
         <v>0.6</v>
       </c>
       <c r="J14">
-        <v>2.1</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
@@ -1108,11 +1171,23 @@
         <v>2.4</v>
       </c>
       <c r="J15">
-        <v>2.2999999999999998</v>
+        <v>1.7</v>
       </c>
       <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
@@ -1141,11 +1216,23 @@
         <v>1</v>
       </c>
       <c r="J16">
-        <v>1.7</v>
+        <v>0.8</v>
       </c>
       <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
@@ -1174,11 +1261,23 @@
         <v>0.5</v>
       </c>
       <c r="J17">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>22</v>
       </c>
@@ -1207,11 +1306,23 @@
         <v>0.4</v>
       </c>
       <c r="J18">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="K18" s="2"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
@@ -1240,13 +1351,25 @@
         <v>1</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="K19" s="2"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>1</v>
@@ -1273,7 +1396,19 @@
         <v>0.3</v>
       </c>
       <c r="J20">
-        <v>0.7</v>
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1283,490 +1418,45 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81D16BE7-6C90-4074-8461-776E5BAB972F}">
-  <dimension ref="A1:G22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB716688-D00E-4DF1-A7D3-BFA4390A64E4}">
+  <dimension ref="B1:K1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C1" t="s">
+      <c r="K1" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="D1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3">
-        <v>0.49299999999999999</v>
-      </c>
-      <c r="C3">
-        <v>0.69299999999999995</v>
-      </c>
-      <c r="D3">
-        <v>7.8</v>
-      </c>
-      <c r="E3">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="F3">
-        <v>1.8</v>
-      </c>
-      <c r="G3">
-        <v>25.3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4">
-        <v>0.503</v>
-      </c>
-      <c r="C4">
-        <v>0.84599999999999997</v>
-      </c>
-      <c r="D4">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="E4">
-        <v>3.2</v>
-      </c>
-      <c r="F4">
-        <v>2.5</v>
-      </c>
-      <c r="G4">
-        <v>26.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5">
-        <v>0.46700000000000003</v>
-      </c>
-      <c r="C5">
-        <v>0.77500000000000002</v>
-      </c>
-      <c r="D5">
-        <v>2.1</v>
-      </c>
-      <c r="E5">
-        <v>1.6</v>
-      </c>
-      <c r="F5">
-        <v>1.9</v>
-      </c>
-      <c r="G5">
-        <v>9.3000000000000007</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6">
-        <v>0.436</v>
-      </c>
-      <c r="C6">
-        <v>0.73499999999999999</v>
-      </c>
-      <c r="D6">
-        <v>4.5</v>
-      </c>
-      <c r="E6">
-        <v>1.3</v>
-      </c>
-      <c r="F6">
-        <v>2.1</v>
-      </c>
-      <c r="G6">
-        <v>12.8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7">
-        <v>0.41599999999999998</v>
-      </c>
-      <c r="C7">
-        <v>0.68799999999999994</v>
-      </c>
-      <c r="D7">
-        <v>3.3</v>
-      </c>
-      <c r="E7">
-        <v>1.3</v>
-      </c>
-      <c r="F7">
-        <v>2</v>
-      </c>
-      <c r="G7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8">
-        <v>0.44400000000000001</v>
-      </c>
-      <c r="C8">
-        <v>0.83299999999999996</v>
-      </c>
-      <c r="D8">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="E8">
-        <v>1.3</v>
-      </c>
-      <c r="F8">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="G8">
-        <v>8.6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9">
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="C9">
-        <v>0.875</v>
-      </c>
-      <c r="D9">
-        <v>1.9</v>
-      </c>
-      <c r="E9">
-        <v>2.4</v>
-      </c>
-      <c r="F9">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="G9">
-        <v>11.9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10">
-        <v>0.41799999999999998</v>
-      </c>
-      <c r="C10">
-        <v>0.65900000000000003</v>
-      </c>
-      <c r="D10">
-        <v>3</v>
-      </c>
-      <c r="E10">
-        <v>5</v>
-      </c>
-      <c r="F10">
-        <v>1.2</v>
-      </c>
-      <c r="G10">
-        <v>7.1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11">
-        <v>0.72899999999999998</v>
-      </c>
-      <c r="C11">
-        <v>0.51400000000000001</v>
-      </c>
-      <c r="D11">
-        <v>7.3</v>
-      </c>
-      <c r="E11">
-        <v>0.7</v>
-      </c>
-      <c r="F11">
-        <v>3.2</v>
-      </c>
-      <c r="G11">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12">
-        <v>0.41199999999999998</v>
-      </c>
-      <c r="C12">
-        <v>0.73399999999999999</v>
-      </c>
-      <c r="D12">
-        <v>1.9</v>
-      </c>
-      <c r="E12">
-        <v>1.9</v>
-      </c>
-      <c r="F12">
-        <v>1.5</v>
-      </c>
-      <c r="G12">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13">
-        <v>0.63700000000000001</v>
-      </c>
-      <c r="C13">
-        <v>0.64600000000000002</v>
-      </c>
-      <c r="D13">
-        <v>5.7</v>
-      </c>
-      <c r="E13">
-        <v>0.5</v>
-      </c>
-      <c r="F13">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="G13">
-        <v>6.6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14">
-        <v>0.40600000000000003</v>
-      </c>
-      <c r="C14">
-        <v>0.83299999999999996</v>
-      </c>
-      <c r="D14">
-        <v>3.2</v>
-      </c>
-      <c r="E14">
-        <v>0.6</v>
-      </c>
-      <c r="F14">
-        <v>2.1</v>
-      </c>
-      <c r="G14">
-        <v>5.3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15">
-        <v>0.46700000000000003</v>
-      </c>
-      <c r="C15">
-        <v>0.5</v>
-      </c>
-      <c r="D15">
-        <v>1.2</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15">
-        <v>1.7</v>
-      </c>
-      <c r="G15">
-        <v>5.7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16">
-        <v>0.318</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>0.8</v>
-      </c>
-      <c r="E16">
-        <v>0.5</v>
-      </c>
-      <c r="F16">
-        <v>0.8</v>
-      </c>
-      <c r="G16">
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17">
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="C17">
-        <v>0.78600000000000003</v>
-      </c>
-      <c r="D17">
-        <v>1.2</v>
-      </c>
-      <c r="E17">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F17">
-        <v>0.6</v>
-      </c>
-      <c r="G17">
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18">
-        <v>0.39200000000000002</v>
-      </c>
-      <c r="C18">
-        <v>0.625</v>
-      </c>
-      <c r="D18">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E18">
-        <v>0.3</v>
-      </c>
-      <c r="F18">
-        <v>0.7</v>
-      </c>
-      <c r="G18">
-        <v>4.2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19">
-        <v>0.5</v>
-      </c>
-      <c r="D19">
-        <v>5</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20">
-        <v>0.4</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>1.2</v>
-      </c>
-      <c r="E20">
-        <v>0.6</v>
-      </c>
-      <c r="F20">
-        <v>0.9</v>
-      </c>
-      <c r="G20">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>56</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <v>0.5</v>
-      </c>
-      <c r="D21">
-        <v>0.6</v>
-      </c>
-      <c r="E21">
-        <v>0.4</v>
-      </c>
-      <c r="F21">
-        <v>0.4</v>
-      </c>
-      <c r="G21">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>57</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0.5</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added functioning lakers api route
</commit_message>
<xml_diff>
--- a/Players.xlsx
+++ b/Players.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDB2139-1D21-468A-8BA7-17F6E561B2A9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15EF31F2-6621-49C5-A929-53E17ADEFC9F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="44">
   <si>
     <t>Kentavious Caldwell-Pope</t>
   </si>
@@ -505,7 +505,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,9 +514,12 @@
     <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" customWidth="1"/>
+    <col min="13" max="13" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="6" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="4.28515625" bestFit="1" customWidth="1"/>
@@ -555,6 +558,15 @@
       </c>
       <c r="K1" s="2" t="s">
         <v>34</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated table syntax for Raptors/Heat
</commit_message>
<xml_diff>
--- a/Players.xlsx
+++ b/Players.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBBA156-6BC8-44E0-AB63-DED68A42E683}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17849A0B-93D7-49DF-B588-A2C18AA3B3CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2925" yWindow="0" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rockets" sheetId="6" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="212">
   <si>
     <t>Kentavious Caldwell-Pope</t>
   </si>
@@ -318,9 +318,6 @@
     <t>dragigo01</t>
   </si>
   <si>
-    <t>Goran DragiÄ‡</t>
-  </si>
-  <si>
     <t>crowdja01</t>
   </si>
   <si>
@@ -402,12 +399,6 @@
     <t>KZ Okpala</t>
   </si>
   <si>
-    <t>maconda01</t>
-  </si>
-  <si>
-    <t>Daryl Macon</t>
-  </si>
-  <si>
     <t>lowryky01</t>
   </si>
   <si>
@@ -510,12 +501,6 @@
     <t>Dewan Hernandez</t>
   </si>
   <si>
-    <t>pondssh01</t>
-  </si>
-  <si>
-    <t>Shamorie Ponds</t>
-  </si>
-  <si>
     <t>hardeja01</t>
   </si>
   <si>
@@ -700,6 +685,27 @@
   </si>
   <si>
     <t>Zach Norvell</t>
+  </si>
+  <si>
+    <t>Goran Dragic</t>
+  </si>
+  <si>
+    <t>6'9</t>
+  </si>
+  <si>
+    <t>6'2</t>
+  </si>
+  <si>
+    <t>6'11</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>turnovers</t>
   </si>
 </sst>
 </file>
@@ -862,8 +868,8 @@
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_2" connectionId="4" xr16:uid="{4601FA81-F96F-4FCE-BD0D-CD03933565EA}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="29">
-    <queryTableFields count="28">
+  <queryTableRefresh nextId="34" unboundColumnsRight="5">
+    <queryTableFields count="33">
       <queryTableField id="1" name="pID" tableColumnId="1"/>
       <queryTableField id="2" name="Column1" tableColumnId="2"/>
       <queryTableField id="3" name="Age" tableColumnId="3"/>
@@ -892,6 +898,11 @@
       <queryTableField id="26" name="TOV" tableColumnId="26"/>
       <queryTableField id="27" name="PF" tableColumnId="27"/>
       <queryTableField id="28" name="PTS/G" tableColumnId="28"/>
+      <queryTableField id="29" dataBound="0" tableColumnId="29"/>
+      <queryTableField id="30" dataBound="0" tableColumnId="30"/>
+      <queryTableField id="31" dataBound="0" tableColumnId="31"/>
+      <queryTableField id="32" dataBound="0" tableColumnId="32"/>
+      <queryTableField id="33" dataBound="0" tableColumnId="33"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
@@ -899,8 +910,8 @@
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="2" xr16:uid="{B9156521-B171-4AC7-B073-4101935ACDF1}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="29">
-    <queryTableFields count="28">
+  <queryTableRefresh nextId="34" unboundColumnsRight="5">
+    <queryTableFields count="33">
       <queryTableField id="1" name="pID" tableColumnId="1"/>
       <queryTableField id="2" name="Name" tableColumnId="2"/>
       <queryTableField id="3" name="Age" tableColumnId="3"/>
@@ -929,6 +940,11 @@
       <queryTableField id="26" name="TOV" tableColumnId="26"/>
       <queryTableField id="27" name="PF" tableColumnId="27"/>
       <queryTableField id="28" name="PTS/G" tableColumnId="28"/>
+      <queryTableField id="29" dataBound="0" tableColumnId="29"/>
+      <queryTableField id="30" dataBound="0" tableColumnId="30"/>
+      <queryTableField id="31" dataBound="0" tableColumnId="31"/>
+      <queryTableField id="32" dataBound="0" tableColumnId="32"/>
+      <queryTableField id="33" dataBound="0" tableColumnId="33"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
@@ -942,8 +958,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0F4EF9E5-9677-43A8-A736-865594885CFA}" name="Rockets" displayName="Rockets" ref="A1:AB22" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:AB22" xr:uid="{4B57AF0C-9BDD-4BD8-83D7-B10EB0C9603A}"/>
   <tableColumns count="28">
-    <tableColumn id="1" xr3:uid="{3A970909-7651-4ECD-8DAC-5C48EB9A9B10}" uniqueName="1" name="pID" queryTableFieldId="1" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{54DD752A-DFEF-4F59-ABFF-3A306542E0A9}" uniqueName="2" name="Name" queryTableFieldId="2" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{3A970909-7651-4ECD-8DAC-5C48EB9A9B10}" uniqueName="1" name="pID" queryTableFieldId="1" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{54DD752A-DFEF-4F59-ABFF-3A306542E0A9}" uniqueName="2" name="Name" queryTableFieldId="2" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{849BCA9C-C6F4-4E86-BD09-908FC3B80632}" uniqueName="3" name="Age" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{AFB30A1D-7BD2-4AC2-AA02-B5C4EB47FCAF}" uniqueName="4" name="G" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{717CA3D5-0744-4517-9EDD-1193CD50BA36}" uniqueName="5" name="GS" queryTableFieldId="5"/>
@@ -979,8 +995,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{128D8679-3244-4813-9C2D-2CA9AACC5725}" name="Lakers" displayName="Lakers" ref="A1:AB21" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:AB21" xr:uid="{5CEC451F-3C12-4357-85E0-017ABCA60D64}"/>
   <tableColumns count="28">
-    <tableColumn id="1" xr3:uid="{D9BB7FD0-4424-4B5D-918E-268CFF50D955}" uniqueName="1" name="pID" queryTableFieldId="1" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{FFF5DB0B-8F32-4EF9-970A-3AF1118DAC40}" uniqueName="2" name="Name" queryTableFieldId="2" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{D9BB7FD0-4424-4B5D-918E-268CFF50D955}" uniqueName="1" name="pID" queryTableFieldId="1" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{FFF5DB0B-8F32-4EF9-970A-3AF1118DAC40}" uniqueName="2" name="Name" queryTableFieldId="2" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{DA395927-E86B-434A-8CD0-CD41787BA56E}" uniqueName="3" name="Age" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{3A0287DB-091A-413A-9DCB-664BAC1F6F92}" uniqueName="4" name="G" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{1FA51D1F-E3BD-4E4D-97B3-28B5E38A3D93}" uniqueName="5" name="GS" queryTableFieldId="5"/>
@@ -1013,18 +1029,18 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DA21639A-3744-49DC-98E8-C4E303866ECB}" name="Raptors" displayName="Raptors" ref="A1:AB19" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:AB19" xr:uid="{AE867AE2-D4F9-4E63-8F68-B51DF058F583}"/>
-  <tableColumns count="28">
-    <tableColumn id="1" xr3:uid="{5E0D5FFF-58E8-4FE6-817B-1B6FF8ABC20C}" uniqueName="1" name="pID" queryTableFieldId="1" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{1066CC70-B348-49AE-854A-A48F59EF7905}" uniqueName="2" name="Name" queryTableFieldId="2" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{9FEBFD83-B8BA-4892-8223-6495004D2F54}" uniqueName="3" name="Age" queryTableFieldId="3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DA21639A-3744-49DC-98E8-C4E303866ECB}" name="Raptors" displayName="Raptors" ref="A1:AG19" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:AG19" xr:uid="{AE867AE2-D4F9-4E63-8F68-B51DF058F583}"/>
+  <tableColumns count="33">
+    <tableColumn id="1" xr3:uid="{5E0D5FFF-58E8-4FE6-817B-1B6FF8ABC20C}" uniqueName="1" name="pID" queryTableFieldId="1" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{1066CC70-B348-49AE-854A-A48F59EF7905}" uniqueName="2" name="name" queryTableFieldId="2" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{9FEBFD83-B8BA-4892-8223-6495004D2F54}" uniqueName="3" name="age" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{0366A523-BB89-4716-99A6-DCDEBC91E31B}" uniqueName="4" name="G" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{D6D59391-510D-421B-92F8-F80C14CCF551}" uniqueName="5" name="GS" queryTableFieldId="5"/>
     <tableColumn id="6" xr3:uid="{78BAD14F-AAEB-4ADE-8E0C-C02F09135FEE}" uniqueName="6" name="MP" queryTableFieldId="6"/>
     <tableColumn id="7" xr3:uid="{0DBF3C81-A658-442B-8500-D1F495FA960B}" uniqueName="7" name="FG" queryTableFieldId="7"/>
     <tableColumn id="8" xr3:uid="{EE6E1102-CDF0-4BEB-B07D-719C75C667BF}" uniqueName="8" name="FGA" queryTableFieldId="8"/>
-    <tableColumn id="9" xr3:uid="{0226FDD0-E4D1-46CC-9825-8108BBD17976}" uniqueName="9" name="FG%" queryTableFieldId="9"/>
+    <tableColumn id="9" xr3:uid="{0226FDD0-E4D1-46CC-9825-8108BBD17976}" uniqueName="9" name="fieldgoal" queryTableFieldId="9"/>
     <tableColumn id="10" xr3:uid="{9EBB6101-1663-4CBB-AA85-C0D46885C168}" uniqueName="10" name="3P" queryTableFieldId="10"/>
     <tableColumn id="11" xr3:uid="{5D89989C-5A4D-4A60-86B1-DE0D7C92B92E}" uniqueName="11" name="3PA" queryTableFieldId="11"/>
     <tableColumn id="12" xr3:uid="{BEB8B5F7-D315-4EA7-9141-CCECD6435CE1}" uniqueName="12" name="3P%" queryTableFieldId="12"/>
@@ -1037,31 +1053,36 @@
     <tableColumn id="19" xr3:uid="{4CED1E01-128E-4DE0-962E-A5DE443E8F9D}" uniqueName="19" name="FT%" queryTableFieldId="19"/>
     <tableColumn id="20" xr3:uid="{CE6E6812-B49B-435C-AD30-0C1C795914D4}" uniqueName="20" name="ORB" queryTableFieldId="20"/>
     <tableColumn id="21" xr3:uid="{F2AD3B95-0206-44F4-9763-60BA52DD72A5}" uniqueName="21" name="DRB" queryTableFieldId="21"/>
-    <tableColumn id="22" xr3:uid="{1FA5AC1A-FA21-4EB5-A75D-47CE6C9B5D9D}" uniqueName="22" name="TRB" queryTableFieldId="22"/>
-    <tableColumn id="23" xr3:uid="{D2AAB5D1-9869-47D5-9ECA-ECA2315E9D58}" uniqueName="23" name="AST" queryTableFieldId="23"/>
+    <tableColumn id="22" xr3:uid="{1FA5AC1A-FA21-4EB5-A75D-47CE6C9B5D9D}" uniqueName="22" name="rebounds" queryTableFieldId="22"/>
+    <tableColumn id="23" xr3:uid="{D2AAB5D1-9869-47D5-9ECA-ECA2315E9D58}" uniqueName="23" name="assists" queryTableFieldId="23"/>
     <tableColumn id="24" xr3:uid="{36D233A4-C3D4-44D0-9B07-6A41E6695A3B}" uniqueName="24" name="STL" queryTableFieldId="24"/>
     <tableColumn id="25" xr3:uid="{FC9B3B1B-E552-446B-A083-E84D121FA11D}" uniqueName="25" name="BLK" queryTableFieldId="25"/>
-    <tableColumn id="26" xr3:uid="{0CBCB62E-9057-4E53-AB70-2FC4704021B0}" uniqueName="26" name="TOV" queryTableFieldId="26"/>
-    <tableColumn id="27" xr3:uid="{E482912A-4FBF-45FA-927B-F00F7C672EDA}" uniqueName="27" name="PF" queryTableFieldId="27"/>
+    <tableColumn id="26" xr3:uid="{0CBCB62E-9057-4E53-AB70-2FC4704021B0}" uniqueName="26" name="turnovers" queryTableFieldId="26"/>
+    <tableColumn id="27" xr3:uid="{E482912A-4FBF-45FA-927B-F00F7C672EDA}" uniqueName="27" name="personalfouls" queryTableFieldId="27"/>
     <tableColumn id="28" xr3:uid="{64D9E675-020D-4EDF-AB3D-0FD449EDBC41}" uniqueName="28" name="PTS/G" queryTableFieldId="28"/>
+    <tableColumn id="29" xr3:uid="{F8739A03-FCB5-480F-A75B-C8CF4DDEEED9}" uniqueName="29" name="jersey" queryTableFieldId="29"/>
+    <tableColumn id="30" xr3:uid="{4E79679D-D4DE-4B8D-8395-F4AAC5A55333}" uniqueName="30" name="position" queryTableFieldId="30"/>
+    <tableColumn id="31" xr3:uid="{57886DE0-5A21-4036-9E69-A9AD1C4532C2}" uniqueName="31" name="height" queryTableFieldId="31"/>
+    <tableColumn id="32" xr3:uid="{4BC85C51-B61B-4EAA-9540-F32C2AC55BC9}" uniqueName="32" name="weight" queryTableFieldId="32"/>
+    <tableColumn id="33" xr3:uid="{E7B1D8F4-7C26-4921-A407-7F511826C8E1}" uniqueName="33" name="image" queryTableFieldId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F5A90E02-5C7C-4A78-B1E6-59E99625EC84}" name="Heat" displayName="Heat" ref="A1:AB22" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:AB22" xr:uid="{4521CB1D-070F-4C02-A42D-98363EE30D91}"/>
-  <tableColumns count="28">
-    <tableColumn id="1" xr3:uid="{0984C9ED-1617-46F0-B5CE-707762B2F860}" uniqueName="1" name="pID" queryTableFieldId="1" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{3475D47F-4F74-4283-8A5B-BA79D451AF9A}" uniqueName="2" name="Name" queryTableFieldId="2" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{D06C076B-DA40-43E3-B82A-4A81AD206CBD}" uniqueName="3" name="Age" queryTableFieldId="3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F5A90E02-5C7C-4A78-B1E6-59E99625EC84}" name="Heat" displayName="Heat" ref="A1:AG22" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:AG22" xr:uid="{4521CB1D-070F-4C02-A42D-98363EE30D91}"/>
+  <tableColumns count="33">
+    <tableColumn id="1" xr3:uid="{0984C9ED-1617-46F0-B5CE-707762B2F860}" uniqueName="1" name="pID" queryTableFieldId="1" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{3475D47F-4F74-4283-8A5B-BA79D451AF9A}" uniqueName="2" name="name" queryTableFieldId="2" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{D06C076B-DA40-43E3-B82A-4A81AD206CBD}" uniqueName="3" name="age" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{9B1AC8F2-AEE9-45F7-B43A-8E7B67D46EC3}" uniqueName="4" name="G" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{0B8F7257-C000-441C-A747-43EF5B886423}" uniqueName="5" name="GS" queryTableFieldId="5"/>
     <tableColumn id="6" xr3:uid="{A3E0BDEC-0E78-43F3-B429-987ACFC860C8}" uniqueName="6" name="MP" queryTableFieldId="6"/>
     <tableColumn id="7" xr3:uid="{C0C0B100-7360-4823-9CDD-746F9FE37A90}" uniqueName="7" name="FG" queryTableFieldId="7"/>
     <tableColumn id="8" xr3:uid="{0733A94F-C52F-4FF4-A4D2-513D48B3D57A}" uniqueName="8" name="FGA" queryTableFieldId="8"/>
-    <tableColumn id="9" xr3:uid="{726A2CDA-9038-4132-9A34-59E9EF8861C0}" uniqueName="9" name="FG%" queryTableFieldId="9"/>
+    <tableColumn id="9" xr3:uid="{726A2CDA-9038-4132-9A34-59E9EF8861C0}" uniqueName="9" name="fieldgoal" queryTableFieldId="9"/>
     <tableColumn id="10" xr3:uid="{BF0A951F-DA72-46DC-B43B-9FE5AB00C59B}" uniqueName="10" name="3P" queryTableFieldId="10"/>
     <tableColumn id="11" xr3:uid="{32DD1591-9083-463D-9F94-7C5A44B68533}" uniqueName="11" name="3PA" queryTableFieldId="11"/>
     <tableColumn id="12" xr3:uid="{0D786875-05D5-4610-AC21-DB2964956CAD}" uniqueName="12" name="3P%" queryTableFieldId="12"/>
@@ -1074,13 +1095,18 @@
     <tableColumn id="19" xr3:uid="{4E3F49A1-F03A-4627-8E50-8B4CFAD94A01}" uniqueName="19" name="FT%" queryTableFieldId="19"/>
     <tableColumn id="20" xr3:uid="{12448119-D5ED-486A-8FB4-D721DF8A5AAF}" uniqueName="20" name="ORB" queryTableFieldId="20"/>
     <tableColumn id="21" xr3:uid="{D4ED2719-55DC-42AD-85FF-C625483284AB}" uniqueName="21" name="DRB" queryTableFieldId="21"/>
-    <tableColumn id="22" xr3:uid="{263D28B8-9B84-46B6-8A49-EE3EF0838F1F}" uniqueName="22" name="TRB" queryTableFieldId="22"/>
-    <tableColumn id="23" xr3:uid="{BFB96BAA-4CC3-421A-8F87-2CA457E11D0D}" uniqueName="23" name="AST" queryTableFieldId="23"/>
+    <tableColumn id="22" xr3:uid="{263D28B8-9B84-46B6-8A49-EE3EF0838F1F}" uniqueName="22" name="rebounds" queryTableFieldId="22"/>
+    <tableColumn id="23" xr3:uid="{BFB96BAA-4CC3-421A-8F87-2CA457E11D0D}" uniqueName="23" name="assists" queryTableFieldId="23"/>
     <tableColumn id="24" xr3:uid="{3263AD3D-0BA9-41BC-8576-808AA2262CF1}" uniqueName="24" name="STL" queryTableFieldId="24"/>
     <tableColumn id="25" xr3:uid="{5A34091C-B2D8-4DF3-8837-0392C02EB1D0}" uniqueName="25" name="BLK" queryTableFieldId="25"/>
-    <tableColumn id="26" xr3:uid="{212D0A25-CAF0-4F11-B38A-BB737B1FF7F8}" uniqueName="26" name="TOV" queryTableFieldId="26"/>
-    <tableColumn id="27" xr3:uid="{210A8F4C-3C63-42D1-A4F2-CDA3740FCC67}" uniqueName="27" name="PF" queryTableFieldId="27"/>
-    <tableColumn id="28" xr3:uid="{22118406-9DA8-4743-94F4-3D5A803A7435}" uniqueName="28" name="PTS/G" queryTableFieldId="28"/>
+    <tableColumn id="26" xr3:uid="{212D0A25-CAF0-4F11-B38A-BB737B1FF7F8}" uniqueName="26" name="turnovers" queryTableFieldId="26"/>
+    <tableColumn id="27" xr3:uid="{210A8F4C-3C63-42D1-A4F2-CDA3740FCC67}" uniqueName="27" name="personalfouls" queryTableFieldId="27"/>
+    <tableColumn id="28" xr3:uid="{22118406-9DA8-4743-94F4-3D5A803A7435}" uniqueName="28" name="points" queryTableFieldId="28"/>
+    <tableColumn id="29" xr3:uid="{DA14ACA4-852D-49A1-B81A-02E94CF77463}" uniqueName="29" name="jersey" queryTableFieldId="29"/>
+    <tableColumn id="30" xr3:uid="{71E84603-A512-4668-8789-2BD942909E22}" uniqueName="30" name="position" queryTableFieldId="30"/>
+    <tableColumn id="31" xr3:uid="{721F9207-3E0B-4531-84D8-E64C37AB754C}" uniqueName="31" name="height" queryTableFieldId="31"/>
+    <tableColumn id="32" xr3:uid="{CC1C4283-C64F-4B9F-A0C0-13856C8F37C3}" uniqueName="32" name="weight" queryTableFieldId="32"/>
+    <tableColumn id="33" xr3:uid="{7365FF5B-7B29-4399-9A29-CE5761777857}" uniqueName="33" name="image" queryTableFieldId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1472,10 +1498,10 @@
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C2">
         <v>30</v>
@@ -1558,10 +1584,10 @@
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C3">
         <v>31</v>
@@ -1644,10 +1670,10 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C4">
         <v>34</v>
@@ -1730,10 +1756,10 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C5">
         <v>29</v>
@@ -1816,10 +1842,10 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C6">
         <v>25</v>
@@ -1899,10 +1925,10 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C7">
         <v>26</v>
@@ -1985,10 +2011,10 @@
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C8">
         <v>31</v>
@@ -2071,10 +2097,10 @@
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C9">
         <v>27</v>
@@ -2157,10 +2183,10 @@
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C10">
         <v>26</v>
@@ -2243,10 +2269,10 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C11">
         <v>33</v>
@@ -2329,10 +2355,10 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C12">
         <v>33</v>
@@ -2415,10 +2441,10 @@
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C13">
         <v>25</v>
@@ -2501,10 +2527,10 @@
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C14">
         <v>21</v>
@@ -2587,10 +2613,10 @@
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C15">
         <v>25</v>
@@ -2673,10 +2699,10 @@
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C16">
         <v>35</v>
@@ -2759,10 +2785,10 @@
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C17">
         <v>22</v>
@@ -2845,10 +2871,10 @@
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C18">
         <v>37</v>
@@ -2928,10 +2954,10 @@
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C19">
         <v>33</v>
@@ -3014,10 +3040,10 @@
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C20">
         <v>31</v>
@@ -3097,10 +3123,10 @@
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C21">
         <v>26</v>
@@ -3177,10 +3203,10 @@
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C22">
         <v>24</v>
@@ -3273,7 +3299,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F81B35C8-5A5E-4142-A1A0-575B7DCE545E}">
   <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3394,7 +3420,7 @@
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
@@ -3480,7 +3506,7 @@
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
@@ -3566,7 +3592,7 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>0</v>
@@ -3652,7 +3678,7 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
@@ -3738,7 +3764,7 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
@@ -3824,7 +3850,7 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>10</v>
@@ -3910,7 +3936,7 @@
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>15</v>
@@ -3996,7 +4022,7 @@
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>11</v>
@@ -4082,7 +4108,7 @@
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>3</v>
@@ -4168,7 +4194,7 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>7</v>
@@ -4254,7 +4280,7 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>5</v>
@@ -4340,7 +4366,7 @@
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>14</v>
@@ -4426,7 +4452,7 @@
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>16</v>
@@ -4512,7 +4538,7 @@
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>17</v>
@@ -4598,7 +4624,7 @@
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>13</v>
@@ -4684,7 +4710,7 @@
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>43</v>
@@ -4770,7 +4796,7 @@
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>23</v>
@@ -4850,7 +4876,7 @@
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>12</v>
@@ -4936,7 +4962,7 @@
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>22</v>
@@ -5019,10 +5045,10 @@
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C21">
         <v>22</v>
@@ -5107,10 +5133,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D7E80A5-CE6F-44C8-B62F-7435AAC76EA5}">
-  <dimension ref="A1:AB19"/>
+  <dimension ref="A1:AG19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5144,15 +5170,15 @@
     <col min="28" max="28" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>44</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>209</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>210</v>
       </c>
       <c r="D1" t="s">
         <v>47</v>
@@ -5170,7 +5196,7 @@
         <v>51</v>
       </c>
       <c r="I1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="J1" t="s">
         <v>53</v>
@@ -5209,10 +5235,10 @@
         <v>64</v>
       </c>
       <c r="V1" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="W1" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="X1" t="s">
         <v>67</v>
@@ -5221,21 +5247,36 @@
         <v>68</v>
       </c>
       <c r="Z1" t="s">
-        <v>69</v>
+        <v>211</v>
       </c>
       <c r="AA1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="AB1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C2">
         <v>33</v>
@@ -5315,13 +5356,25 @@
       <c r="AB2">
         <v>19.399999999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC2">
+        <v>7</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C3">
         <v>25</v>
@@ -5401,13 +5454,25 @@
       <c r="AB3">
         <v>17.600000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC3">
+        <v>23</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C4">
         <v>25</v>
@@ -5487,13 +5552,25 @@
       <c r="AB4">
         <v>22.9</v>
       </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC4">
+        <v>43</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>206</v>
+      </c>
+      <c r="AF4">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C5">
         <v>22</v>
@@ -5573,13 +5650,25 @@
       <c r="AB5">
         <v>10.6</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC5">
+        <v>3</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF5">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C6">
         <v>26</v>
@@ -5659,13 +5748,25 @@
       <c r="AB6">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC6">
+        <v>24</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF6">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C7">
         <v>30</v>
@@ -5745,13 +5846,25 @@
       <c r="AB7">
         <v>15.4</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC7">
+        <v>9</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF7">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C8">
         <v>35</v>
@@ -5831,13 +5944,25 @@
       <c r="AB8">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC8">
+        <v>33</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>208</v>
+      </c>
+      <c r="AF8">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C9">
         <v>24</v>
@@ -5917,13 +6042,25 @@
       <c r="AB9">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC9">
+        <v>22</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF9">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C10">
         <v>25</v>
@@ -6003,13 +6140,25 @@
       <c r="AB10">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC10">
+        <v>4</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF10">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C11">
         <v>22</v>
@@ -6089,13 +6238,25 @@
       <c r="AB11">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF11">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C12">
         <v>27</v>
@@ -6175,13 +6336,25 @@
       <c r="AB12">
         <v>6.6</v>
       </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC12">
+        <v>25</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>206</v>
+      </c>
+      <c r="AF12">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C13">
         <v>25</v>
@@ -6261,13 +6434,25 @@
       <c r="AB13">
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC13">
+        <v>21</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF13">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C14">
         <v>25</v>
@@ -6347,13 +6532,25 @@
       <c r="AB14">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC14">
+        <v>1</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF14">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C15">
         <v>21</v>
@@ -6433,13 +6630,25 @@
       <c r="AB15">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC15">
+        <v>12</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF15">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C16">
         <v>23</v>
@@ -6519,13 +6728,25 @@
       <c r="AB16">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC16">
+        <v>5</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF16">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C17">
         <v>26</v>
@@ -6605,13 +6826,25 @@
       <c r="AB17">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC17">
+        <v>13</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF17">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C18">
         <v>23</v>
@@ -6691,92 +6924,22 @@
       <c r="AB18">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C19">
-        <v>21</v>
-      </c>
-      <c r="D19">
-        <v>4</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>2.8</v>
-      </c>
-      <c r="G19">
-        <v>0.8</v>
-      </c>
-      <c r="H19">
-        <v>1.3</v>
-      </c>
-      <c r="I19">
-        <v>0.6</v>
-      </c>
-      <c r="J19">
-        <v>0.3</v>
-      </c>
-      <c r="K19">
-        <v>0.5</v>
-      </c>
-      <c r="L19">
-        <v>0.5</v>
-      </c>
-      <c r="M19">
-        <v>0.5</v>
-      </c>
-      <c r="N19">
-        <v>0.8</v>
-      </c>
-      <c r="O19">
-        <v>0.66700000000000004</v>
-      </c>
-      <c r="P19">
-        <v>0.7</v>
-      </c>
-      <c r="Q19">
-        <v>0.5</v>
-      </c>
-      <c r="R19">
-        <v>0.5</v>
-      </c>
-      <c r="S19">
-        <v>1</v>
-      </c>
-      <c r="T19">
-        <v>0</v>
-      </c>
-      <c r="U19">
-        <v>0.3</v>
-      </c>
-      <c r="V19">
-        <v>0.3</v>
-      </c>
-      <c r="W19">
-        <v>0.5</v>
-      </c>
-      <c r="X19">
-        <v>0</v>
-      </c>
-      <c r="Y19">
-        <v>0.3</v>
-      </c>
-      <c r="Z19">
-        <v>0</v>
-      </c>
-      <c r="AA19">
-        <v>0.5</v>
-      </c>
-      <c r="AB19">
-        <v>2.2999999999999998</v>
-      </c>
+      <c r="AC18">
+        <v>20</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF18">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6788,10 +6951,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE4B353D-2F2E-4F98-BAD9-01A3B8AF5EBC}">
-  <dimension ref="A1:AB22"/>
+  <dimension ref="A1:AG22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AJ10" sqref="AJ10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6825,15 +6988,15 @@
     <col min="28" max="28" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>44</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>209</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>210</v>
       </c>
       <c r="D1" t="s">
         <v>47</v>
@@ -6851,7 +7014,7 @@
         <v>51</v>
       </c>
       <c r="I1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="J1" t="s">
         <v>53</v>
@@ -6890,10 +7053,10 @@
         <v>64</v>
       </c>
       <c r="V1" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="W1" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="X1" t="s">
         <v>67</v>
@@ -6902,16 +7065,31 @@
         <v>68</v>
       </c>
       <c r="Z1" t="s">
-        <v>69</v>
+        <v>211</v>
       </c>
       <c r="AA1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="AB1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>71</v>
       </c>
@@ -6996,8 +7174,20 @@
       <c r="AB2">
         <v>19.899999999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC2">
+        <v>22</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF2">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>73</v>
       </c>
@@ -7082,8 +7272,20 @@
       <c r="AB3">
         <v>15.9</v>
       </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC3">
+        <v>13</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>206</v>
+      </c>
+      <c r="AF3">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>75</v>
       </c>
@@ -7168,8 +7370,20 @@
       <c r="AB4">
         <v>11.3</v>
       </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC4">
+        <v>20</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF4">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>77</v>
       </c>
@@ -7254,8 +7468,20 @@
       <c r="AB5">
         <v>13.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC5">
+        <v>55</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF5">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>79</v>
       </c>
@@ -7340,13 +7566,25 @@
       <c r="AB6">
         <v>15.3</v>
       </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC6">
+        <v>25</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>207</v>
+      </c>
+      <c r="AF6">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>82</v>
+        <v>205</v>
       </c>
       <c r="C7">
         <v>33</v>
@@ -7426,13 +7664,25 @@
       <c r="AB7">
         <v>16.2</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC7">
+        <v>7</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF7">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="C8">
         <v>29</v>
@@ -7512,13 +7762,25 @@
       <c r="AB8">
         <v>11.9</v>
       </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC8">
+        <v>99</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF8">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="C9">
         <v>20</v>
@@ -7598,13 +7860,25 @@
       <c r="AB9">
         <v>13.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC9">
+        <v>14</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF9">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="C10">
         <v>22</v>
@@ -7684,13 +7958,25 @@
       <c r="AB10">
         <v>8.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC10">
+        <v>5</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF10">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="C11">
         <v>27</v>
@@ -7770,13 +8056,25 @@
       <c r="AB11">
         <v>6.1</v>
       </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF11">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="C12">
         <v>36</v>
@@ -7856,13 +8154,25 @@
       <c r="AB12">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC12">
+        <v>28</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF12">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="C13">
         <v>28</v>
@@ -7942,13 +8252,25 @@
       <c r="AB13">
         <v>8.1999999999999993</v>
       </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC13">
+        <v>9</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>208</v>
+      </c>
+      <c r="AF13">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="C14">
         <v>28</v>
@@ -8028,13 +8350,25 @@
       <c r="AB14">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC14">
+        <v>44</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF14">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="C15">
         <v>32</v>
@@ -8114,10 +8448,22 @@
       <c r="AB15">
         <v>5.7</v>
       </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC15">
+        <v>16</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF15">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>15</v>
@@ -8200,13 +8546,25 @@
       <c r="AB16">
         <v>9.3000000000000007</v>
       </c>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC16">
+        <v>11</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF16">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="C17">
         <v>39</v>
@@ -8286,13 +8644,25 @@
       <c r="AB17">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC17">
+        <v>40</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF17">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="C18">
         <v>23</v>
@@ -8369,13 +8739,25 @@
       <c r="AB18">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC18">
+        <v>2</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF18">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="C19">
         <v>23</v>
@@ -8455,13 +8837,25 @@
       <c r="AB19">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC19">
+        <v>30</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF19">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="C20">
         <v>23</v>
@@ -8535,13 +8929,25 @@
       <c r="AB20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC20">
+        <v>17</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>208</v>
+      </c>
+      <c r="AF20">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>109</v>
       </c>
       <c r="C21">
         <v>20</v>
@@ -8621,89 +9027,22 @@
       <c r="AB21">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C22">
-        <v>24</v>
-      </c>
-      <c r="D22">
+      <c r="AC21">
         <v>4</v>
       </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>3.5</v>
-      </c>
-      <c r="G22">
-        <v>0.3</v>
-      </c>
-      <c r="H22">
-        <v>0.8</v>
-      </c>
-      <c r="I22">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="J22">
-        <v>0.3</v>
-      </c>
-      <c r="K22">
-        <v>0.5</v>
-      </c>
-      <c r="L22">
-        <v>0.5</v>
-      </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
-      <c r="N22">
-        <v>0.3</v>
-      </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
-      <c r="P22">
-        <v>0.5</v>
-      </c>
-      <c r="Q22">
-        <v>0</v>
-      </c>
-      <c r="R22">
-        <v>0</v>
-      </c>
-      <c r="T22">
-        <v>0</v>
-      </c>
-      <c r="U22">
-        <v>0</v>
-      </c>
-      <c r="V22">
-        <v>0</v>
-      </c>
-      <c r="W22">
-        <v>0.3</v>
-      </c>
-      <c r="X22">
-        <v>0</v>
-      </c>
-      <c r="Y22">
-        <v>0</v>
-      </c>
-      <c r="Z22">
-        <v>0.5</v>
-      </c>
-      <c r="AA22">
-        <v>0.3</v>
-      </c>
-      <c r="AB22">
-        <v>0.8</v>
-      </c>
+      <c r="AD21" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF21">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added models and seed files
</commit_message>
<xml_diff>
--- a/Players.xlsx
+++ b/Players.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBBA156-6BC8-44E0-AB63-DED68A42E683}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01E5638-76EC-4D6B-8AD9-DFA02463C69E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2925" yWindow="0" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rockets" sheetId="6" r:id="rId1"/>
@@ -15,25 +15,16 @@
     <sheet name="Lakers" sheetId="1" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="asdad" localSheetId="4">Lakers!$N$1:$S$21</definedName>
+    <definedName name="asdad" localSheetId="4">Lakers!$N$1:$P$21</definedName>
     <definedName name="ExternalData_1" localSheetId="3" hidden="1">Heat!$A$1:$AB$22</definedName>
-    <definedName name="ExternalData_2" localSheetId="2" hidden="1">'Raptors'!$A$1:$AB$19</definedName>
+    <definedName name="ExternalData_2" localSheetId="2" hidden="1">Raptors!$A$1:$AB$19</definedName>
     <definedName name="ExternalData_3" localSheetId="1" hidden="1">'Lakers(2)'!$A$1:$AB$21</definedName>
-    <definedName name="ExternalData_3" localSheetId="0" hidden="1">'Rockets'!$A$1:$AB$22</definedName>
+    <definedName name="ExternalData_3" localSheetId="0" hidden="1">Rockets!$A$1:$AB$22</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -70,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="214">
   <si>
     <t>Kentavious Caldwell-Pope</t>
   </si>
@@ -700,6 +691,18 @@
   </si>
   <si>
     <t>Zach Norvell</t>
+  </si>
+  <si>
+    <t>5'9</t>
+  </si>
+  <si>
+    <t>6'9</t>
+  </si>
+  <si>
+    <t>turnovers</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -788,8 +791,8 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_3" connectionId="5" xr16:uid="{26345376-2E25-45BF-B0E1-3215EE0E4B80}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="29">
-    <queryTableFields count="28">
+  <queryTableRefresh nextId="34" unboundColumnsRight="5">
+    <queryTableFields count="33">
       <queryTableField id="1" name="pID" tableColumnId="1"/>
       <queryTableField id="2" name="Name" tableColumnId="2"/>
       <queryTableField id="3" name="Age" tableColumnId="3"/>
@@ -818,6 +821,11 @@
       <queryTableField id="26" name="TOV" tableColumnId="26"/>
       <queryTableField id="27" name="PF" tableColumnId="27"/>
       <queryTableField id="28" name="PTS/G" tableColumnId="28"/>
+      <queryTableField id="29" dataBound="0" tableColumnId="29"/>
+      <queryTableField id="30" dataBound="0" tableColumnId="30"/>
+      <queryTableField id="31" dataBound="0" tableColumnId="31"/>
+      <queryTableField id="32" dataBound="0" tableColumnId="32"/>
+      <queryTableField id="33" dataBound="0" tableColumnId="33"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
@@ -939,18 +947,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0F4EF9E5-9677-43A8-A736-865594885CFA}" name="Rockets" displayName="Rockets" ref="A1:AB22" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:AB22" xr:uid="{4B57AF0C-9BDD-4BD8-83D7-B10EB0C9603A}"/>
-  <tableColumns count="28">
-    <tableColumn id="1" xr3:uid="{3A970909-7651-4ECD-8DAC-5C48EB9A9B10}" uniqueName="1" name="pID" queryTableFieldId="1" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{54DD752A-DFEF-4F59-ABFF-3A306542E0A9}" uniqueName="2" name="Name" queryTableFieldId="2" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0F4EF9E5-9677-43A8-A736-865594885CFA}" name="Rockets" displayName="Rockets" ref="A1:AG22" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:AG22" xr:uid="{4B57AF0C-9BDD-4BD8-83D7-B10EB0C9603A}"/>
+  <tableColumns count="33">
+    <tableColumn id="1" xr3:uid="{3A970909-7651-4ECD-8DAC-5C48EB9A9B10}" uniqueName="1" name="pID" queryTableFieldId="1" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{54DD752A-DFEF-4F59-ABFF-3A306542E0A9}" uniqueName="2" name="name" queryTableFieldId="2" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{849BCA9C-C6F4-4E86-BD09-908FC3B80632}" uniqueName="3" name="Age" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{AFB30A1D-7BD2-4AC2-AA02-B5C4EB47FCAF}" uniqueName="4" name="G" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{717CA3D5-0744-4517-9EDD-1193CD50BA36}" uniqueName="5" name="GS" queryTableFieldId="5"/>
     <tableColumn id="6" xr3:uid="{D349F419-9BCD-422A-B8BD-A84AD26A9A33}" uniqueName="6" name="MP" queryTableFieldId="6"/>
     <tableColumn id="7" xr3:uid="{176F2EAD-3EAE-43C7-9E87-D76192C27AC4}" uniqueName="7" name="FG" queryTableFieldId="7"/>
     <tableColumn id="8" xr3:uid="{DF6E1957-8C7F-478F-9586-2B117D9E6094}" uniqueName="8" name="FGA" queryTableFieldId="8"/>
-    <tableColumn id="9" xr3:uid="{718531B2-87E0-478C-B047-08A5FB9EF518}" uniqueName="9" name="FG%" queryTableFieldId="9"/>
+    <tableColumn id="9" xr3:uid="{718531B2-87E0-478C-B047-08A5FB9EF518}" uniqueName="9" name="fieldgoal" queryTableFieldId="9"/>
     <tableColumn id="10" xr3:uid="{E4E55324-B3F3-4AD2-A638-E7FF4F65E142}" uniqueName="10" name="3P" queryTableFieldId="10"/>
     <tableColumn id="11" xr3:uid="{4E6F92A9-398C-4195-8E06-2A8A10185535}" uniqueName="11" name="3PA" queryTableFieldId="11"/>
     <tableColumn id="12" xr3:uid="{D0857FF0-D728-407A-9846-F4065DC25182}" uniqueName="12" name="3P%" queryTableFieldId="12"/>
@@ -963,13 +971,18 @@
     <tableColumn id="19" xr3:uid="{DE50592D-2A7D-42A8-9570-0E6DB261D62D}" uniqueName="19" name="FT%" queryTableFieldId="19"/>
     <tableColumn id="20" xr3:uid="{888E90E0-3346-4359-A07F-5E89BE7853B3}" uniqueName="20" name="ORB" queryTableFieldId="20"/>
     <tableColumn id="21" xr3:uid="{24F79FEB-D244-40D5-BD42-3D2B92D26F7B}" uniqueName="21" name="DRB" queryTableFieldId="21"/>
-    <tableColumn id="22" xr3:uid="{8B91521A-9539-43BA-9487-ECA446337F2D}" uniqueName="22" name="TRB" queryTableFieldId="22"/>
-    <tableColumn id="23" xr3:uid="{6607D095-1114-4F23-B16A-3DE549E3DC3B}" uniqueName="23" name="AST" queryTableFieldId="23"/>
+    <tableColumn id="22" xr3:uid="{8B91521A-9539-43BA-9487-ECA446337F2D}" uniqueName="22" name="rebounds" queryTableFieldId="22"/>
+    <tableColumn id="23" xr3:uid="{6607D095-1114-4F23-B16A-3DE549E3DC3B}" uniqueName="23" name="assists" queryTableFieldId="23"/>
     <tableColumn id="24" xr3:uid="{723D8E07-61AD-4ED2-9FE5-89A1FCF11732}" uniqueName="24" name="STL" queryTableFieldId="24"/>
     <tableColumn id="25" xr3:uid="{84E3DBF3-4053-414C-BD94-0B90E4A43C1E}" uniqueName="25" name="BLK" queryTableFieldId="25"/>
-    <tableColumn id="26" xr3:uid="{428EA063-D795-46AC-886A-B31D91E4409B}" uniqueName="26" name="TOV" queryTableFieldId="26"/>
-    <tableColumn id="27" xr3:uid="{50639BA6-1073-4370-AF46-E9FCAC70669C}" uniqueName="27" name="PF" queryTableFieldId="27"/>
-    <tableColumn id="28" xr3:uid="{73A5092E-35F8-44A3-9486-4522E6718335}" uniqueName="28" name="PTS/G" queryTableFieldId="28"/>
+    <tableColumn id="26" xr3:uid="{428EA063-D795-46AC-886A-B31D91E4409B}" uniqueName="26" name="turnovers" queryTableFieldId="26"/>
+    <tableColumn id="27" xr3:uid="{50639BA6-1073-4370-AF46-E9FCAC70669C}" uniqueName="27" name="personalfouls" queryTableFieldId="27"/>
+    <tableColumn id="28" xr3:uid="{73A5092E-35F8-44A3-9486-4522E6718335}" uniqueName="28" name="points" queryTableFieldId="28"/>
+    <tableColumn id="29" xr3:uid="{BD3E1ACF-74DD-4EDB-A9F1-BBE3D1F33B0B}" uniqueName="29" name="jersey" queryTableFieldId="29"/>
+    <tableColumn id="30" xr3:uid="{511E669A-7BAD-40D8-B856-D6A0192A51DC}" uniqueName="30" name="position" queryTableFieldId="30"/>
+    <tableColumn id="31" xr3:uid="{0AD85919-64BE-4279-8A41-8F929330F09F}" uniqueName="31" name="height" queryTableFieldId="31"/>
+    <tableColumn id="32" xr3:uid="{1B06A364-440B-433A-9AB9-7F93F1CF208E}" uniqueName="32" name="weight" queryTableFieldId="32"/>
+    <tableColumn id="33" xr3:uid="{145159E1-625E-4AA6-B1E5-3E8F3F7A66CA}" uniqueName="33" name="image" queryTableFieldId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -979,8 +992,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{128D8679-3244-4813-9C2D-2CA9AACC5725}" name="Lakers" displayName="Lakers" ref="A1:AB21" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:AB21" xr:uid="{5CEC451F-3C12-4357-85E0-017ABCA60D64}"/>
   <tableColumns count="28">
-    <tableColumn id="1" xr3:uid="{D9BB7FD0-4424-4B5D-918E-268CFF50D955}" uniqueName="1" name="pID" queryTableFieldId="1" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{FFF5DB0B-8F32-4EF9-970A-3AF1118DAC40}" uniqueName="2" name="Name" queryTableFieldId="2" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{D9BB7FD0-4424-4B5D-918E-268CFF50D955}" uniqueName="1" name="pID" queryTableFieldId="1" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{FFF5DB0B-8F32-4EF9-970A-3AF1118DAC40}" uniqueName="2" name="Name" queryTableFieldId="2" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{DA395927-E86B-434A-8CD0-CD41787BA56E}" uniqueName="3" name="Age" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{3A0287DB-091A-413A-9DCB-664BAC1F6F92}" uniqueName="4" name="G" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{1FA51D1F-E3BD-4E4D-97B3-28B5E38A3D93}" uniqueName="5" name="GS" queryTableFieldId="5"/>
@@ -1016,8 +1029,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DA21639A-3744-49DC-98E8-C4E303866ECB}" name="Raptors" displayName="Raptors" ref="A1:AB19" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:AB19" xr:uid="{AE867AE2-D4F9-4E63-8F68-B51DF058F583}"/>
   <tableColumns count="28">
-    <tableColumn id="1" xr3:uid="{5E0D5FFF-58E8-4FE6-817B-1B6FF8ABC20C}" uniqueName="1" name="pID" queryTableFieldId="1" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{1066CC70-B348-49AE-854A-A48F59EF7905}" uniqueName="2" name="Name" queryTableFieldId="2" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{5E0D5FFF-58E8-4FE6-817B-1B6FF8ABC20C}" uniqueName="1" name="pID" queryTableFieldId="1" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{1066CC70-B348-49AE-854A-A48F59EF7905}" uniqueName="2" name="Name" queryTableFieldId="2" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{9FEBFD83-B8BA-4892-8223-6495004D2F54}" uniqueName="3" name="Age" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{0366A523-BB89-4716-99A6-DCDEBC91E31B}" uniqueName="4" name="G" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{D6D59391-510D-421B-92F8-F80C14CCF551}" uniqueName="5" name="GS" queryTableFieldId="5"/>
@@ -1053,8 +1066,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F5A90E02-5C7C-4A78-B1E6-59E99625EC84}" name="Heat" displayName="Heat" ref="A1:AB22" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:AB22" xr:uid="{4521CB1D-070F-4C02-A42D-98363EE30D91}"/>
   <tableColumns count="28">
-    <tableColumn id="1" xr3:uid="{0984C9ED-1617-46F0-B5CE-707762B2F860}" uniqueName="1" name="pID" queryTableFieldId="1" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{3475D47F-4F74-4283-8A5B-BA79D451AF9A}" uniqueName="2" name="Name" queryTableFieldId="2" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{0984C9ED-1617-46F0-B5CE-707762B2F860}" uniqueName="1" name="pID" queryTableFieldId="1" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{3475D47F-4F74-4283-8A5B-BA79D451AF9A}" uniqueName="2" name="Name" queryTableFieldId="2" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{D06C076B-DA40-43E3-B82A-4A81AD206CBD}" uniqueName="3" name="Age" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{9B1AC8F2-AEE9-45F7-B43A-8E7B67D46EC3}" uniqueName="4" name="G" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{0B8F7257-C000-441C-A747-43EF5B886423}" uniqueName="5" name="GS" queryTableFieldId="5"/>
@@ -1349,47 +1362,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3049898-9159-4D1C-802A-7336A35BC27B}">
-  <dimension ref="A1:AB22"/>
+  <dimension ref="A1:AG22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="AF9" sqref="AF9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="7" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="6.7109375" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="7" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="5.42578125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="7" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="8.42578125" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="5.28515625" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="6.5703125" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="6.85546875" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="7" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="6.85546875" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.5703125" customWidth="1"/>
+    <col min="24" max="24" width="6.140625" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="6.42578125" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="7" customWidth="1"/>
+    <col min="27" max="27" width="5.42578125" customWidth="1"/>
+    <col min="28" max="28" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>44</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>213</v>
       </c>
       <c r="C1" t="s">
         <v>46</v>
@@ -1410,7 +1426,7 @@
         <v>51</v>
       </c>
       <c r="I1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="J1" t="s">
         <v>53</v>
@@ -1449,10 +1465,10 @@
         <v>64</v>
       </c>
       <c r="V1" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="W1" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="X1" t="s">
         <v>67</v>
@@ -1461,16 +1477,31 @@
         <v>68</v>
       </c>
       <c r="Z1" t="s">
-        <v>69</v>
+        <v>212</v>
       </c>
       <c r="AA1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="AB1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>148</v>
       </c>
@@ -1555,8 +1586,20 @@
       <c r="AB2">
         <v>34.299999999999997</v>
       </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC2">
+        <v>13</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>150</v>
       </c>
@@ -1641,8 +1684,20 @@
       <c r="AB3">
         <v>27.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>152</v>
       </c>
@@ -1727,8 +1782,20 @@
       <c r="AB4">
         <v>6.9</v>
       </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC4">
+        <v>17</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF4">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>154</v>
       </c>
@@ -1813,8 +1880,20 @@
       <c r="AB5">
         <v>11.6</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC5">
+        <v>33</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF5">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>156</v>
       </c>
@@ -1896,8 +1975,20 @@
       <c r="AB6">
         <v>13.9</v>
       </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC6">
+        <v>15</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF6">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>158</v>
       </c>
@@ -1982,8 +2073,20 @@
       <c r="AB7">
         <v>10.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC7">
+        <v>4</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF7">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>160</v>
       </c>
@@ -2068,8 +2171,20 @@
       <c r="AB8">
         <v>14.4</v>
       </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC8">
+        <v>10</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF8">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>162</v>
       </c>
@@ -2154,8 +2269,20 @@
       <c r="AB9">
         <v>8.8000000000000007</v>
       </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC9">
+        <v>25</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF9">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>164</v>
       </c>
@@ -2240,8 +2367,20 @@
       <c r="AB10">
         <v>10.1</v>
       </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC10">
+        <v>16</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF10">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>166</v>
       </c>
@@ -2326,8 +2465,20 @@
       <c r="AB11">
         <v>12.2</v>
       </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC11">
+        <v>32</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF11">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>168</v>
       </c>
@@ -2412,8 +2563,20 @@
       <c r="AB12">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC12">
+        <v>9</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF12">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>170</v>
       </c>
@@ -2498,8 +2661,20 @@
       <c r="AB13">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC13">
+        <v>12</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF13">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>172</v>
       </c>
@@ -2584,8 +2759,20 @@
       <c r="AB14">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC14">
+        <v>55</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF14">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>174</v>
       </c>
@@ -2670,8 +2857,20 @@
       <c r="AB15">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC15">
+        <v>21</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF15">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>176</v>
       </c>
@@ -2756,8 +2955,20 @@
       <c r="AB16">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC16">
+        <v>18</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF16">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>178</v>
       </c>
@@ -2842,8 +3053,20 @@
       <c r="AB17">
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC17">
+        <v>3</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>210</v>
+      </c>
+      <c r="AF17">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>180</v>
       </c>
@@ -2925,8 +3148,20 @@
       <c r="AB18">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC18">
+        <v>19</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF18">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>182</v>
       </c>
@@ -3011,8 +3246,20 @@
       <c r="AB19">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC19">
+        <v>12</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF19">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>184</v>
       </c>
@@ -3094,8 +3341,20 @@
       <c r="AB20">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC20">
+        <v>33</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>211</v>
+      </c>
+      <c r="AF20">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>186</v>
       </c>
@@ -3174,8 +3433,20 @@
       <c r="AB21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC21">
+        <v>52</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF21">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>188</v>
       </c>
@@ -3259,6 +3530,18 @@
       </c>
       <c r="AB22">
         <v>3.5</v>
+      </c>
+      <c r="AC22">
+        <v>5</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>211</v>
+      </c>
+      <c r="AF22">
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -3273,37 +3556,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F81B35C8-5A5E-4142-A1A0-575B7DCE545E}">
   <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" customWidth="1"/>
+    <col min="8" max="8" width="7" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" customWidth="1"/>
+    <col min="11" max="11" width="6.7109375" customWidth="1"/>
+    <col min="12" max="12" width="7" customWidth="1"/>
+    <col min="13" max="13" width="5.42578125" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" customWidth="1"/>
+    <col min="15" max="15" width="7" customWidth="1"/>
+    <col min="16" max="16" width="8.42578125" customWidth="1"/>
+    <col min="17" max="17" width="5.28515625" customWidth="1"/>
+    <col min="18" max="18" width="6.5703125" customWidth="1"/>
+    <col min="19" max="19" width="6.85546875" customWidth="1"/>
+    <col min="20" max="20" width="7" customWidth="1"/>
+    <col min="21" max="21" width="6.85546875" customWidth="1"/>
+    <col min="22" max="23" width="6.5703125" customWidth="1"/>
+    <col min="24" max="24" width="6.140625" customWidth="1"/>
+    <col min="25" max="25" width="6.42578125" customWidth="1"/>
     <col min="26" max="26" width="7" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.42578125" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="8.7109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -5110,7 +5395,7 @@
   <dimension ref="A1:AB19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="Z1" sqref="Z1:Z1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6791,7 +7076,7 @@
   <dimension ref="A1:AB22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8715,33 +9000,34 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" customWidth="1"/>
-    <col min="13" max="13" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" customWidth="1"/>
+    <col min="15" max="15" width="6.7109375" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>213</v>
+      </c>
       <c r="B1" s="2" t="s">
         <v>42</v>
       </c>
@@ -8770,19 +9056,22 @@
         <v>33</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -8813,21 +9102,24 @@
       <c r="J2">
         <v>1.9</v>
       </c>
-      <c r="K2" s="2"/>
-      <c r="L2">
+      <c r="K2">
+        <v>0.9</v>
+      </c>
+      <c r="L2" s="2"/>
+      <c r="N2">
         <f>ROUNDUP(H2,0)*10</f>
         <v>30</v>
       </c>
-      <c r="M2">
+      <c r="O2">
         <f>ROUNDUP(I2,0)*10</f>
         <v>20</v>
       </c>
-      <c r="N2">
+      <c r="P2">
         <f>ROUNDUP(J2,0)*10</f>
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -8858,21 +9150,24 @@
       <c r="J3">
         <v>3.2</v>
       </c>
-      <c r="K3" s="2"/>
-      <c r="L3">
-        <f t="shared" ref="L3:L20" si="0">ROUNDUP(H3,0)*10</f>
+      <c r="K3">
+        <v>1.2</v>
+      </c>
+      <c r="L3" s="2"/>
+      <c r="N3">
+        <f>ROUNDUP(H3,0)*10</f>
         <v>80</v>
       </c>
-      <c r="M3">
-        <f t="shared" ref="M3:M20" si="1">ROUNDUP(I3,0)*10</f>
+      <c r="O3">
+        <f>ROUNDUP(I3,0)*10</f>
         <v>10</v>
       </c>
-      <c r="N3">
-        <f t="shared" ref="N3:N20" si="2">ROUNDUP(J3,0)*10</f>
+      <c r="P3">
+        <f>ROUNDUP(J3,0)*10</f>
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -8903,21 +9198,24 @@
       <c r="J4">
         <v>2.2999999999999998</v>
       </c>
-      <c r="K4" s="2"/>
-      <c r="L4">
-        <f t="shared" si="0"/>
+      <c r="K4">
+        <v>0.9</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="N4">
+        <f>ROUNDUP(H4,0)*10</f>
         <v>40</v>
       </c>
-      <c r="M4">
-        <f t="shared" si="1"/>
+      <c r="O4">
+        <f>ROUNDUP(I4,0)*10</f>
         <v>20</v>
       </c>
-      <c r="N4">
-        <f t="shared" si="2"/>
+      <c r="P4">
+        <f>ROUNDUP(J4,0)*10</f>
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -8948,21 +9246,24 @@
       <c r="J5">
         <v>1.8</v>
       </c>
-      <c r="K5" s="2"/>
-      <c r="L5">
-        <f t="shared" si="0"/>
+      <c r="K5">
+        <v>0.8</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="N5">
+        <f>ROUNDUP(H5,0)*10</f>
         <v>60</v>
       </c>
-      <c r="M5">
-        <f t="shared" si="1"/>
+      <c r="O5">
+        <f>ROUNDUP(I5,0)*10</f>
         <v>10</v>
       </c>
-      <c r="N5">
-        <f t="shared" si="2"/>
+      <c r="P5">
+        <f>ROUNDUP(J5,0)*10</f>
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -8993,21 +9294,24 @@
       <c r="J6">
         <v>1.5</v>
       </c>
-      <c r="K6" s="2"/>
-      <c r="L6">
-        <f t="shared" si="0"/>
+      <c r="K6">
+        <v>3.9</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="N6">
+        <f>ROUNDUP(H6,0)*10</f>
         <v>80</v>
       </c>
-      <c r="M6">
-        <f t="shared" si="1"/>
+      <c r="O6">
+        <f>ROUNDUP(I6,0)*10</f>
         <v>110</v>
       </c>
-      <c r="N6">
-        <f t="shared" si="2"/>
+      <c r="P6">
+        <f>ROUNDUP(J6,0)*10</f>
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -9038,21 +9342,24 @@
       <c r="J7">
         <v>2.5</v>
       </c>
-      <c r="K7" s="2"/>
-      <c r="L7">
-        <f t="shared" si="0"/>
+      <c r="K7">
+        <v>0.8</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="N7">
+        <f>ROUNDUP(H7,0)*10</f>
         <v>20</v>
       </c>
-      <c r="M7">
-        <f t="shared" si="1"/>
+      <c r="O7">
+        <f>ROUNDUP(I7,0)*10</f>
         <v>20</v>
       </c>
-      <c r="N7">
-        <f t="shared" si="2"/>
+      <c r="P7">
+        <f>ROUNDUP(J7,0)*10</f>
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -9083,21 +9390,24 @@
       <c r="J8">
         <v>2.1</v>
       </c>
-      <c r="K8" s="2"/>
-      <c r="L8">
-        <f t="shared" si="0"/>
+      <c r="K8">
+        <v>2.5</v>
+      </c>
+      <c r="L8" s="2"/>
+      <c r="N8">
+        <f>ROUNDUP(H8,0)*10</f>
         <v>100</v>
       </c>
-      <c r="M8">
-        <f t="shared" si="1"/>
+      <c r="O8">
+        <f>ROUNDUP(I8,0)*10</f>
         <v>40</v>
       </c>
-      <c r="N8">
-        <f t="shared" si="2"/>
+      <c r="P8">
+        <f>ROUNDUP(J8,0)*10</f>
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -9128,21 +9438,24 @@
       <c r="J9">
         <v>2.2000000000000002</v>
       </c>
-      <c r="K9" s="2"/>
-      <c r="L9">
-        <f t="shared" si="0"/>
+      <c r="K9">
+        <v>1.5</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="N9">
+        <f>ROUNDUP(H9,0)*10</f>
         <v>50</v>
       </c>
-      <c r="M9">
-        <f t="shared" si="1"/>
+      <c r="O9">
+        <f>ROUNDUP(I9,0)*10</f>
         <v>20</v>
       </c>
-      <c r="N9">
-        <f t="shared" si="2"/>
+      <c r="P9">
+        <f>ROUNDUP(J9,0)*10</f>
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -9173,21 +9486,24 @@
       <c r="J10">
         <v>1.2</v>
       </c>
-      <c r="K10" s="2"/>
-      <c r="L10">
-        <f t="shared" si="0"/>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10" s="2"/>
+      <c r="N10">
+        <f>ROUNDUP(H10,0)*10</f>
         <v>30</v>
       </c>
-      <c r="M10">
-        <f t="shared" si="1"/>
+      <c r="O10">
+        <f>ROUNDUP(I10,0)*10</f>
         <v>20</v>
       </c>
-      <c r="N10">
-        <f t="shared" si="2"/>
+      <c r="P10">
+        <f>ROUNDUP(J10,0)*10</f>
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -9218,21 +9534,24 @@
       <c r="J11">
         <v>0.9</v>
       </c>
-      <c r="K11" s="2"/>
-      <c r="L11">
-        <f t="shared" si="0"/>
+      <c r="K11">
+        <v>1.9</v>
+      </c>
+      <c r="L11" s="2"/>
+      <c r="N11">
+        <f>ROUNDUP(H11,0)*10</f>
         <v>30</v>
       </c>
-      <c r="M11">
-        <f t="shared" si="1"/>
+      <c r="O11">
+        <f>ROUNDUP(I11,0)*10</f>
         <v>50</v>
       </c>
-      <c r="N11">
-        <f t="shared" si="2"/>
+      <c r="P11">
+        <f>ROUNDUP(J11,0)*10</f>
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
@@ -9263,21 +9582,24 @@
       <c r="J12">
         <v>0.6</v>
       </c>
-      <c r="K12" s="2"/>
-      <c r="L12">
-        <f t="shared" si="0"/>
+      <c r="K12">
+        <v>0.2</v>
+      </c>
+      <c r="L12" s="2"/>
+      <c r="N12">
+        <f>ROUNDUP(H12,0)*10</f>
         <v>20</v>
       </c>
-      <c r="M12">
-        <f t="shared" si="1"/>
+      <c r="O12">
+        <f>ROUNDUP(I12,0)*10</f>
         <v>10</v>
       </c>
-      <c r="N12">
-        <f t="shared" si="2"/>
+      <c r="P12">
+        <f>ROUNDUP(J12,0)*10</f>
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -9308,21 +9630,24 @@
       <c r="J13">
         <v>2.1</v>
       </c>
-      <c r="K13" s="2"/>
-      <c r="L13">
-        <f t="shared" si="0"/>
+      <c r="K13">
+        <v>0.8</v>
+      </c>
+      <c r="L13" s="2"/>
+      <c r="N13">
+        <f>ROUNDUP(H13,0)*10</f>
         <v>20</v>
       </c>
-      <c r="M13">
-        <f t="shared" si="1"/>
+      <c r="O13">
+        <f>ROUNDUP(I13,0)*10</f>
         <v>20</v>
       </c>
-      <c r="N13">
-        <f t="shared" si="2"/>
+      <c r="P13">
+        <f>ROUNDUP(J13,0)*10</f>
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
@@ -9353,21 +9678,24 @@
       <c r="J14">
         <v>2.2999999999999998</v>
       </c>
-      <c r="K14" s="2"/>
-      <c r="L14">
-        <f t="shared" si="0"/>
+      <c r="K14">
+        <v>0.4</v>
+      </c>
+      <c r="L14" s="2"/>
+      <c r="N14">
+        <f>ROUNDUP(H14,0)*10</f>
         <v>40</v>
       </c>
-      <c r="M14">
-        <f t="shared" si="1"/>
+      <c r="O14">
+        <f>ROUNDUP(I14,0)*10</f>
         <v>10</v>
       </c>
-      <c r="N14">
-        <f t="shared" si="2"/>
+      <c r="P14">
+        <f>ROUNDUP(J14,0)*10</f>
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
@@ -9398,21 +9726,24 @@
       <c r="J15">
         <v>1.7</v>
       </c>
-      <c r="K15" s="2"/>
-      <c r="L15">
-        <f t="shared" si="0"/>
+      <c r="K15">
+        <v>1.9</v>
+      </c>
+      <c r="L15" s="2"/>
+      <c r="N15">
+        <f>ROUNDUP(H15,0)*10</f>
         <v>20</v>
       </c>
-      <c r="M15">
-        <f t="shared" si="1"/>
+      <c r="O15">
+        <f>ROUNDUP(I15,0)*10</f>
         <v>30</v>
       </c>
-      <c r="N15">
-        <f t="shared" si="2"/>
+      <c r="P15">
+        <f>ROUNDUP(J15,0)*10</f>
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
@@ -9443,21 +9774,24 @@
       <c r="J16">
         <v>0.8</v>
       </c>
-      <c r="K16" s="2"/>
-      <c r="L16">
-        <f t="shared" si="0"/>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16" s="2"/>
+      <c r="N16">
+        <f>ROUNDUP(H16,0)*10</f>
         <v>20</v>
       </c>
-      <c r="M16">
-        <f t="shared" si="1"/>
+      <c r="O16">
+        <f>ROUNDUP(I16,0)*10</f>
         <v>10</v>
       </c>
-      <c r="N16">
-        <f t="shared" si="2"/>
+      <c r="P16">
+        <f>ROUNDUP(J16,0)*10</f>
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
@@ -9488,21 +9822,24 @@
       <c r="J17">
         <v>0.4</v>
       </c>
-      <c r="K17" s="2"/>
-      <c r="L17">
-        <f t="shared" si="0"/>
+      <c r="K17">
+        <v>0.7</v>
+      </c>
+      <c r="L17" s="2"/>
+      <c r="N17">
+        <f>ROUNDUP(H17,0)*10</f>
         <v>10</v>
       </c>
-      <c r="M17">
-        <f t="shared" si="1"/>
+      <c r="O17">
+        <f>ROUNDUP(I17,0)*10</f>
         <v>10</v>
       </c>
-      <c r="N17">
-        <f t="shared" si="2"/>
+      <c r="P17">
+        <f>ROUNDUP(J17,0)*10</f>
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>22</v>
       </c>
@@ -9533,21 +9870,24 @@
       <c r="J18">
         <v>0</v>
       </c>
-      <c r="K18" s="2"/>
-      <c r="L18">
-        <f t="shared" si="0"/>
+      <c r="K18">
+        <v>0.2</v>
+      </c>
+      <c r="L18" s="2"/>
+      <c r="N18">
+        <f>ROUNDUP(H18,0)*10</f>
         <v>10</v>
       </c>
-      <c r="M18">
-        <f t="shared" si="1"/>
+      <c r="O18">
+        <f>ROUNDUP(I18,0)*10</f>
         <v>10</v>
       </c>
-      <c r="N18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P18">
+        <f>ROUNDUP(J18,0)*10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
@@ -9578,21 +9918,24 @@
       <c r="J19">
         <v>0.7</v>
       </c>
-      <c r="K19" s="2"/>
-      <c r="L19">
-        <f t="shared" si="0"/>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2"/>
+      <c r="N19">
+        <f>ROUNDUP(H19,0)*10</f>
         <v>50</v>
       </c>
-      <c r="M19">
-        <f t="shared" si="1"/>
+      <c r="O19">
+        <f>ROUNDUP(I19,0)*10</f>
         <v>10</v>
       </c>
-      <c r="N19">
-        <f t="shared" si="2"/>
+      <c r="P19">
+        <f>ROUNDUP(J19,0)*10</f>
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>43</v>
       </c>
@@ -9623,16 +9966,19 @@
       <c r="J20">
         <v>0</v>
       </c>
-      <c r="L20">
-        <f t="shared" si="0"/>
+      <c r="K20">
+        <v>0.2</v>
+      </c>
+      <c r="N20">
+        <f>ROUNDUP(H20,0)*10</f>
         <v>20</v>
       </c>
-      <c r="M20">
-        <f t="shared" si="1"/>
+      <c r="O20">
+        <f>ROUNDUP(I20,0)*10</f>
         <v>10</v>
       </c>
-      <c r="N20">
-        <f t="shared" si="2"/>
+      <c r="P20">
+        <f>ROUNDUP(J20,0)*10</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>